<commit_message>
update example excel file
</commit_message>
<xml_diff>
--- a/trackhub/test/data/example.xlsx
+++ b/trackhub/test/data/example.xlsx
@@ -5,116 +5,240 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/NICHD-core0/infrastructure/trackhub-cleaned-version/trackhub/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/dalerr/proj/trackhub/trackhub/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCED915-5DEA-E54F-97E3-1006EB22AA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC00E409-560B-7441-B28B-894A3AD22FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6800" yWindow="4740" windowWidth="35760" windowHeight="24060" activeTab="1" xr2:uid="{602047F2-C907-FF4D-A627-A2C80FCB89FF}"/>
+    <workbookView xWindow="6800" yWindow="4740" windowWidth="35760" windowHeight="24060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="1" r:id="rId1"/>
-    <sheet name="bigwigs" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="12" r:id="rId3"/>
-    <sheet name="aggregate_config" sheetId="16" r:id="rId4"/>
-    <sheet name="super_config" sheetId="13" r:id="rId5"/>
-    <sheet name="composite_config" sheetId="4" r:id="rId6"/>
-    <sheet name="Sheet2" sheetId="14" r:id="rId7"/>
-    <sheet name="view_config" sheetId="6" r:id="rId8"/>
-    <sheet name="interact" sheetId="17" r:id="rId9"/>
+    <sheet name="bigwigs" sheetId="2" r:id="rId2"/>
+    <sheet name="aggregate_config" sheetId="4" r:id="rId3"/>
+    <sheet name="super_config" sheetId="5" r:id="rId4"/>
+    <sheet name="composite_config" sheetId="6" r:id="rId5"/>
+    <sheet name="view_config" sheetId="8" r:id="rId6"/>
+    <sheet name="interact" sheetId="9" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="80">
+  <si>
+    <t>hub_name</t>
+  </si>
+  <si>
+    <t>test_excel_to_trackhub</t>
+  </si>
   <si>
     <t>short_label</t>
   </si>
   <si>
+    <t>Test Excel file</t>
+  </si>
+  <si>
     <t>long_label</t>
   </si>
   <si>
+    <t>This is a test for the script that will make a track hub out of any excel file</t>
+  </si>
+  <si>
     <t>email</t>
   </si>
   <si>
+    <t>eva.jason@nih.gov</t>
+  </si>
+  <si>
     <t>genome</t>
   </si>
   <si>
+    <t>hg19</t>
+  </si>
+  <si>
     <t>name</t>
   </si>
   <si>
+    <t>tracktype</t>
+  </si>
+  <si>
+    <t>visibility</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>container</t>
+  </si>
+  <si>
+    <t>container_type</t>
+  </si>
+  <si>
+    <t>dimensions</t>
+  </si>
+  <si>
+    <t>filterComposite</t>
+  </si>
+  <si>
+    <t>subgroup_celltype</t>
+  </si>
+  <si>
+    <t>subgroup_genotype</t>
+  </si>
+  <si>
+    <t>subgroup_treatment</t>
+  </si>
+  <si>
+    <t>subgroup_strand</t>
+  </si>
+  <si>
+    <t>negateValues</t>
+  </si>
+  <si>
+    <t>autoScale</t>
+  </si>
+  <si>
+    <t>bigDataUrl</t>
+  </si>
+  <si>
+    <t>WT_treatment_A_pos</t>
+  </si>
+  <si>
+    <t>bigWig</t>
+  </si>
+  <si>
+    <t>full</t>
+  </si>
+  <si>
+    <t>120,51,154</t>
+  </si>
+  <si>
+    <t>experiment1</t>
+  </si>
+  <si>
     <t>composite</t>
   </si>
   <si>
-    <t>color</t>
-  </si>
-  <si>
-    <t>visibility</t>
-  </si>
-  <si>
-    <t>subgroup_strand</t>
-  </si>
-  <si>
-    <t>negateValues</t>
-  </si>
-  <si>
-    <t>autoScale</t>
-  </si>
-  <si>
-    <t>tracktype</t>
-  </si>
-  <si>
-    <t>full</t>
+    <t>dimX=genotype dimY=treatment dimA=strand</t>
+  </si>
+  <si>
+    <t>dimA</t>
+  </si>
+  <si>
+    <t>WT</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>pos</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>http://genome.ucsc.edu/goldenPath/help/examples/bigWigExample.bw</t>
+  </si>
+  <si>
+    <t>MUT_treatment_A_pos</t>
   </si>
   <si>
     <t>squish</t>
   </si>
   <si>
-    <t>120,51,154</t>
-  </si>
-  <si>
-    <t>subgroup_treatment</t>
-  </si>
-  <si>
-    <t>A</t>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>WT_treatment_A_neg</t>
+  </si>
+  <si>
+    <t>neg</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>MUT_treatment_A_neg</t>
+  </si>
+  <si>
+    <t>WT_treatment_B_pos</t>
   </si>
   <si>
     <t>B</t>
   </si>
   <si>
-    <t>bigWig</t>
+    <t>MUT_treatment_B_pos</t>
+  </si>
+  <si>
+    <t>WT_treatment_B_neg</t>
+  </si>
+  <si>
+    <t>MUT_treatment_B_neg</t>
+  </si>
+  <si>
+    <t>WT_treatment_A_pos2</t>
+  </si>
+  <si>
+    <t>wild_type_pos2</t>
+  </si>
+  <si>
+    <t>view</t>
+  </si>
+  <si>
+    <t>MUT_treatment_A_pos2</t>
+  </si>
+  <si>
+    <t>mutant_pos2</t>
+  </si>
+  <si>
+    <t>WT_treatment_A_neg2</t>
+  </si>
+  <si>
+    <t>wild_type_neg2</t>
+  </si>
+  <si>
+    <t>K562</t>
+  </si>
+  <si>
+    <t>MUT_treatment_A_neg2</t>
+  </si>
+  <si>
+    <t>mutant_neg2</t>
+  </si>
+  <si>
+    <t>WT_treatment_B_pos2</t>
+  </si>
+  <si>
+    <t>MUT_treatment_B_pos2</t>
+  </si>
+  <si>
+    <t>WT_treatment_B_neg2</t>
+  </si>
+  <si>
+    <t>MUT_treatment_B_neg2</t>
+  </si>
+  <si>
+    <t>aggregate</t>
+  </si>
+  <si>
+    <t>agg_track</t>
+  </si>
+  <si>
+    <t>transparentOverlay</t>
   </si>
   <si>
     <t>super_track_1</t>
   </si>
   <si>
-    <t>pos</t>
-  </si>
-  <si>
-    <t>neg</t>
-  </si>
-  <si>
-    <t>on</t>
-  </si>
-  <si>
-    <t>bigBed</t>
+    <t>super</t>
+  </si>
+  <si>
+    <t>experiment2</t>
+  </si>
+  <si>
+    <t>interact</t>
   </si>
   <si>
     <t>regions</t>
@@ -123,215 +247,32 @@
     <t>dense</t>
   </si>
   <si>
-    <t>group</t>
-  </si>
-  <si>
-    <t>denseCoverage</t>
-  </si>
-  <si>
-    <t>38,140,34</t>
-  </si>
-  <si>
-    <t>view</t>
-  </si>
-  <si>
-    <t>test_excel_to_trackhub</t>
-  </si>
-  <si>
-    <t>This is a test for the script that will make a track hub out of any excel file</t>
-  </si>
-  <si>
-    <t>Test Excel file</t>
-  </si>
-  <si>
-    <t>WT_treatment_A_pos</t>
-  </si>
-  <si>
-    <t>MUT_treatment_A_pos</t>
-  </si>
-  <si>
-    <t>WT_treatment_A_neg</t>
-  </si>
-  <si>
-    <t>MUT_treatment_A_neg</t>
-  </si>
-  <si>
-    <t>WT_treatment_B_pos</t>
-  </si>
-  <si>
-    <t>MUT_treatment_B_pos</t>
-  </si>
-  <si>
-    <t>WT_treatment_B_neg</t>
-  </si>
-  <si>
-    <t>MUT_treatment_B_neg</t>
-  </si>
-  <si>
-    <t>experiment1</t>
-  </si>
-  <si>
-    <t>subgroup_genotype</t>
-  </si>
-  <si>
-    <t>super</t>
-  </si>
-  <si>
-    <t>another_track</t>
-  </si>
-  <si>
-    <t>experiment2</t>
-  </si>
-  <si>
-    <t>a_different_track</t>
-  </si>
-  <si>
-    <t>120,51,155</t>
-  </si>
-  <si>
-    <t>120,51,156</t>
-  </si>
-  <si>
-    <t>aggregate</t>
-  </si>
-  <si>
-    <t>agg_track</t>
-  </si>
-  <si>
-    <t>transparentOverlay</t>
-  </si>
-  <si>
-    <t>WT</t>
-  </si>
-  <si>
-    <t>MT</t>
-  </si>
-  <si>
-    <t>WT_treatment_A_pos2</t>
-  </si>
-  <si>
-    <t>MUT_treatment_A_pos2</t>
-  </si>
-  <si>
-    <t>WT_treatment_A_neg2</t>
-  </si>
-  <si>
-    <t>MUT_treatment_A_neg2</t>
-  </si>
-  <si>
-    <t>WT_treatment_B_pos2</t>
-  </si>
-  <si>
-    <t>MUT_treatment_B_pos2</t>
-  </si>
-  <si>
-    <t>WT_treatment_B_neg2</t>
-  </si>
-  <si>
-    <t>MUT_treatment_B_neg2</t>
-  </si>
-  <si>
-    <t>wild_type_pos2</t>
-  </si>
-  <si>
-    <t>mutant_pos2</t>
-  </si>
-  <si>
-    <t>wild_type_neg2</t>
-  </si>
-  <si>
-    <t>mutant_neg2</t>
-  </si>
-  <si>
-    <t>bigDataUrl</t>
-  </si>
-  <si>
-    <t>eva.jason@nih.gov</t>
-  </si>
-  <si>
-    <t>http://genome.ucsc.edu/goldenPath/help/examples/bigWigExample.bw</t>
-  </si>
-  <si>
-    <t>hg19</t>
-  </si>
-  <si>
     <t>bigInteract</t>
   </si>
   <si>
+    <t>shortLabel</t>
+  </si>
+  <si>
+    <t>spectrum</t>
+  </si>
+  <si>
+    <t>scoreMin</t>
+  </si>
+  <si>
+    <t>maxHeightPixels</t>
+  </si>
+  <si>
     <t>http://genome.ucsc.edu/goldenPath/help/examples/interact/interactExample3.inter.bb</t>
   </si>
   <si>
-    <t>shortLabel</t>
-  </si>
-  <si>
-    <t>spectrum</t>
-  </si>
-  <si>
-    <t>scoreMin</t>
-  </si>
-  <si>
-    <t>maxHeightPixels</t>
-  </si>
-  <si>
     <t>300:150:20</t>
-  </si>
-  <si>
-    <t>some_other_track</t>
-  </si>
-  <si>
-    <t>hub_name</t>
-  </si>
-  <si>
-    <t>interact</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>/data/NICHD-core0/infrastructure/trackhub-cleaned-version/trackhub/test/data/random-hg38-0.bigBed</t>
-  </si>
-  <si>
-    <t>test/data/sine-hg38-2.bedgraph.bw</t>
-  </si>
-  <si>
-    <t>test/data/sine-hg38-1.bedgraph.bw</t>
-  </si>
-  <si>
-    <t>test/data/sine-hg38-0.bedgraph.bw</t>
-  </si>
-  <si>
-    <t>container</t>
-  </si>
-  <si>
-    <t>container_type</t>
-  </si>
-  <si>
-    <t>bb</t>
-  </si>
-  <si>
-    <t>dimX=genotype dimY=treatment dimA=strand</t>
-  </si>
-  <si>
-    <t>dimensions</t>
-  </si>
-  <si>
-    <t>filterComposite</t>
-  </si>
-  <si>
-    <t>dimA</t>
-  </si>
-  <si>
-    <t>subgroup_celltype</t>
-  </si>
-  <si>
-    <t>K562</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -343,12 +284,6 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -400,15 +335,15 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -723,7 +658,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF633367-F76D-2241-94D9-564DFC40E354}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -732,58 +667,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{D68CBC32-5B1B-8A42-BD8C-E9F9282C7DCD}"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9B3F100-C897-D745-B32E-ACB5482B2D6E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -804,421 +739,421 @@
   <sheetData>
     <row r="1" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>90</v>
+        <v>17</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="M2" s="5"/>
       <c r="N2" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="M6" s="5"/>
       <c r="N6" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="M7" s="3"/>
       <c r="N7" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1228,30 +1163,30 @@
       <c r="L10" s="3"/>
       <c r="M10" s="5"/>
       <c r="N10" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1261,104 +1196,104 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="F12" s="3" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="5" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1368,30 +1303,30 @@
       <c r="L14" s="3"/>
       <c r="M14" s="5"/>
       <c r="N14" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1401,30 +1336,30 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -1433,33 +1368,33 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="5" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -1468,90 +1403,22 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8350D90-F2FA-2E45-9109-9265388FC26A}">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C8D6566-AF40-D54C-9CAB-5978C9BC01BF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1562,48 +1429,48 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1611,8 +1478,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{698BC2BA-085F-0A4F-B62E-51B6DC755F83}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1623,24 +1490,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1648,8 +1515,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F22B51BF-C7CA-0848-9D24-4D7F5585E1E5}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScale="267" zoomScaleNormal="267" workbookViewId="0">
@@ -1666,189 +1533,59 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C7C532A-7228-CF49-8B87-6C5B4D025007}">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD2758D-F3BD-FF4F-9AF5-443EE5DB99BD}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1868,150 +1605,149 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
         <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G2" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07554C9A-03CA-E64C-BAB8-3CEFF3949ADC}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2027,71 +1763,71 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I1" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="J1" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="G2">
         <v>175</v>
       </c>
       <c r="H2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{66E155F1-5200-A241-8BE1-9EE9E4FD0FBD}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>